<commit_message>
Add conversion for Yes/No values in input
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F88145A-4A9E-4C1C-83CD-AC3D1907587E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D512592-DA2E-41DC-B55A-1CF593C62B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="114">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>[+/- °]</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -567,7 +570,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -602,6 +605,9 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
@@ -619,434 +625,434 @@
       <font>
         <b/>
         <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
       </font>
     </dxf>
     <dxf>
@@ -1382,8 +1388,8 @@
   </sheetPr>
   <dimension ref="B1:H111"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1408,6 +1414,9 @@
       <c r="B3" s="7" t="s">
         <v>32</v>
       </c>
+      <c r="C3" s="12" t="s">
+        <v>113</v>
+      </c>
       <c r="E3" s="11" t="s">
         <v>94</v>
       </c>
@@ -2076,7 +2085,7 @@
         <v>57</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="106" spans="2:5" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2126,27 +2135,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="cellIs" dxfId="61" priority="67" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="68" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="61" priority="68" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="67" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C12">
-    <cfRule type="cellIs" dxfId="59" priority="65" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="66" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="59" priority="66" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="65" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C15">
-    <cfRule type="cellIs" dxfId="57" priority="63" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="64" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="57" priority="64" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="63" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C18">
@@ -2158,11 +2167,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="cellIs" dxfId="53" priority="59" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="60" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="53" priority="60" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="59" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
@@ -2174,43 +2183,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="49" priority="55" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="56" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="49" priority="56" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="55" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30 C33">
-    <cfRule type="cellIs" dxfId="47" priority="53" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="54" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="47" priority="54" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="53" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="45" priority="51" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="45" priority="52" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="51" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="cellIs" dxfId="43" priority="49" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="50" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="43" priority="50" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="49" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="41" priority="47" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="48" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="41" priority="48" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="47" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
@@ -2222,27 +2231,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="37" priority="43" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="44" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="37" priority="44" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="43" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="cellIs" dxfId="35" priority="41" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="42" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="35" priority="42" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="41" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="33" priority="40" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="39" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
@@ -2254,27 +2263,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="29" priority="36" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="35" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="27" priority="34" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="33" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71">
-    <cfRule type="cellIs" dxfId="25" priority="31" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="32" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="25" priority="32" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="31" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
@@ -2286,43 +2295,43 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="cellIs" dxfId="21" priority="27" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="28" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="21" priority="28" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="27" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C80">
-    <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="25" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83">
-    <cfRule type="cellIs" dxfId="17" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87">
-    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="15" priority="22" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="21" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91:C92">
-    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="20" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="19" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94">
@@ -2334,19 +2343,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="17" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
@@ -2358,19 +2367,19 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C108">
-    <cfRule type="cellIs" dxfId="3" priority="15" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="16" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="16" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="15" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C111">
-    <cfRule type="cellIs" dxfId="1" priority="13" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="14" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="1" priority="14" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -2386,15 +2395,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2540,6 +2540,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2547,14 +2556,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2568,6 +2569,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add required input files for LEGO-GAMS, fix reading-in with new format
Add *.mps and *.opt files to .gitignore
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D512592-DA2E-41DC-B55A-1CF593C62B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4EEA9B-07AA-4325-B52C-FDE8607B10FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5835" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Parameters" sheetId="121" r:id="rId1"/>
@@ -1388,8 +1388,8 @@
   </sheetPr>
   <dimension ref="B1:H111"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2085,7 +2085,7 @@
         <v>57</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106" spans="2:5" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2395,6 +2395,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2540,15 +2549,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2556,6 +2556,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2569,14 +2577,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add pFixStInterResToIniReserve to Power_Parameters
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4EEA9B-07AA-4325-B52C-FDE8607B10FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEED2F2-E81C-4813-9815-0C5D9B5A275B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5835" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="117">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -406,6 +406,15 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>Fix last vStInterRes in last period to IniReserve</t>
+  </si>
+  <si>
+    <t>pFixStInterResToIniReserve</t>
+  </si>
+  <si>
+    <t>Yes: vStInterRes[lastPeriod] == IniReserve, No: vStInterRes[lastPeriod] &gt;= IniReserve</t>
   </si>
 </sst>
 </file>
@@ -620,439 +629,453 @@
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
   </cellStyles>
-  <dxfs count="64">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
+  <dxfs count="66">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
       </font>
     </dxf>
     <dxf>
@@ -1386,10 +1409,10 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:H111"/>
+  <dimension ref="B1:H114"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="E107" sqref="E107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2088,30 +2111,33 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="2:5" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B106" s="7" t="s">
+    <row r="106" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B106" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C106" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B107" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B109" s="7" t="s">
         <v>76</v>
-      </c>
-    </row>
-    <row r="107" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B107" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C107" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="108" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B108" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C108" s="6" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="110" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C110" s="8" t="s">
         <v>56</v>
@@ -2119,271 +2145,287 @@
     </row>
     <row r="111" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B111" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C111" s="6" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="113" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B113" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C113" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B114" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C114" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C6">
-    <cfRule type="cellIs" dxfId="63" priority="7" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="7" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="8" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="cellIs" dxfId="61" priority="68" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="67" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="63" priority="67" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="68" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C12">
-    <cfRule type="cellIs" dxfId="59" priority="66" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="65" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="61" priority="65" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="66" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C15">
-    <cfRule type="cellIs" dxfId="57" priority="64" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="63" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="59" priority="63" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="64" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C18">
-    <cfRule type="cellIs" dxfId="55" priority="61" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="61" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="62" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="cellIs" dxfId="53" priority="60" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="59" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="55" priority="59" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="60" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="cellIs" dxfId="51" priority="77" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="78" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="77" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="78" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="49" priority="56" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="55" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="51" priority="55" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="56" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30 C33">
-    <cfRule type="cellIs" dxfId="47" priority="54" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="53" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="49" priority="53" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="54" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="45" priority="52" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="51" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="47" priority="51" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="52" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="cellIs" dxfId="43" priority="50" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="49" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="45" priority="49" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="50" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="41" priority="48" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="47" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="43" priority="47" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="48" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="45" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="46" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="37" priority="44" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="43" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="39" priority="43" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="44" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C53">
-    <cfRule type="cellIs" dxfId="35" priority="42" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="41" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="37" priority="41" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="42" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="cellIs" dxfId="33" priority="40" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="39" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="35" priority="39" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="40" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="31" priority="37" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="37" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="38" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="29" priority="36" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="35" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="31" priority="35" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="36" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C67">
-    <cfRule type="cellIs" dxfId="27" priority="34" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="33" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="29" priority="33" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="34" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71">
-    <cfRule type="cellIs" dxfId="25" priority="32" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="31" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="27" priority="31" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="32" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="29" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="30" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="cellIs" dxfId="21" priority="28" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="27" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="23" priority="27" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="28" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C80">
-    <cfRule type="cellIs" dxfId="19" priority="26" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="25" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="26" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83">
-    <cfRule type="cellIs" dxfId="17" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="5" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="6" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C87">
-    <cfRule type="cellIs" dxfId="15" priority="22" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="21" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="17" priority="21" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="22" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C91:C92">
-    <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="19" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="15" priority="19" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="20" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="17" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C104">
-    <cfRule type="cellIs" dxfId="5" priority="11" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C108">
-    <cfRule type="cellIs" dxfId="3" priority="16" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="15" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C104 C107">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C111">
-    <cfRule type="cellIs" dxfId="1" priority="14" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="5" priority="15" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="16" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C114">
+    <cfRule type="cellIs" dxfId="3" priority="13" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C24 C27 C36 C49 C53 C71 C87 C98 C108 C111 C104 C91:C92" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C24 C27 C36 C49 C53 C71 C87 C98 C111 C114 C91:C92 C104 C107" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
       <formula1>"No, Yes"</formula1>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C9 C12 C15 C18 C21" xr:uid="{87C6F772-FD4B-9449-B9E7-DA0FF0A031BB}"/>
@@ -2395,15 +2437,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2549,6 +2582,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2556,14 +2598,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2577,6 +2611,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Implement read-in and verification of new Import/Export input files
Adjust Power_Parameters.xlsx with correct information
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E99FDBE-9386-46EE-AD7D-953F1B8D9639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8784CB98-1D2F-44C9-89D1-1257C322C1DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-34572" yWindow="-17508" windowWidth="30936" windowHeight="16776" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Parameters" sheetId="121" r:id="rId1"/>
@@ -423,7 +423,7 @@
     <t>pEnablePowerImportExport</t>
   </si>
   <si>
-    <t>Requires Power_ImpExp.xlsx file</t>
+    <t>Requires Power_ImpExpHubs.xlsx and Power_ImpExpProfiles.xlsx files</t>
   </si>
 </sst>
 </file>
@@ -638,453 +638,439 @@
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
   </cellStyles>
-  <dxfs count="68">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
+  <dxfs count="66">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
       </font>
     </dxf>
     <dxf>
@@ -1435,7 +1421,7 @@
   <dimension ref="B1:H117"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1489,7 +1475,7 @@
         <v>118</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>119</v>
@@ -2214,276 +2200,268 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="cellIs" dxfId="65" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="cellIs" dxfId="67" priority="11" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="11" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="12" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C12">
-    <cfRule type="cellIs" dxfId="65" priority="71" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="72" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="61" priority="72" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="71" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C15">
-    <cfRule type="cellIs" dxfId="63" priority="69" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="70" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="59" priority="70" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="69" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C18">
-    <cfRule type="cellIs" dxfId="61" priority="67" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="67" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="68" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:C21">
-    <cfRule type="cellIs" dxfId="59" priority="65" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="66" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
-    <cfRule type="cellIs" dxfId="57" priority="63" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="66" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="65" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23:C24">
+    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="55" priority="81" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="82" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="51" priority="82" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="81" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C30">
-    <cfRule type="cellIs" dxfId="53" priority="59" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="60" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="49" priority="60" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="59" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33 C36">
-    <cfRule type="cellIs" dxfId="51" priority="57" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="58" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="47" priority="58" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="57" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="cellIs" dxfId="49" priority="55" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="55" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="56" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C42">
-    <cfRule type="cellIs" dxfId="47" priority="53" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="54" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="43" priority="54" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="53" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="cellIs" dxfId="45" priority="51" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="52" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="41" priority="52" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="51" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="43" priority="49" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="50" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="39" priority="50" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="49" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="cellIs" dxfId="41" priority="47" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="47" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="48" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C56">
-    <cfRule type="cellIs" dxfId="39" priority="45" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="46" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="35" priority="46" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="45" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="37" priority="43" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="44" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="33" priority="44" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="43" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62">
-    <cfRule type="cellIs" dxfId="35" priority="41" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="42" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="31" priority="42" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="41" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C65">
-    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="39" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="40" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C70">
-    <cfRule type="cellIs" dxfId="31" priority="37" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="38" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="27" priority="38" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="37" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C74">
-    <cfRule type="cellIs" dxfId="29" priority="35" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="36" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="25" priority="36" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="35" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C77">
-    <cfRule type="cellIs" dxfId="27" priority="33" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="34" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="23" priority="34" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="33" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C80">
-    <cfRule type="cellIs" dxfId="25" priority="31" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="31" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="32" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C83">
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="30" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="19" priority="30" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="29" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C86">
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="9" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C90">
-    <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="15" priority="26" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="25" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C94:C95">
-    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="13" priority="24" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="23" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C97">
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="11" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="5" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101">
-    <cfRule type="cellIs" dxfId="13" priority="21" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="22" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="9" priority="22" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="21" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C104">
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="8" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C107 C110">
-    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="5" priority="16" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="15" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C114">
-    <cfRule type="cellIs" dxfId="7" priority="19" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="20" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="20" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="19" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C117">
-    <cfRule type="cellIs" dxfId="5" priority="17" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="18" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="1" priority="18" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="17" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -2508,6 +2486,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2653,12 +2637,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
@@ -2668,6 +2646,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2683,20 +2677,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix missing existing lines due
Set pMinFirmCap in Power_Parameters == 0 to remove FirmCap-Constraints
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3666A930-8174-4C26-978C-8126ACA565E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A364A49D-B683-4149-9EB9-E8252B16C13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1420,9 +1420,7 @@
   </sheetPr>
   <dimension ref="B1:H117"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1918,7 +1916,7 @@
         <v>19</v>
       </c>
       <c r="C70" s="10">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="2:3" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -2477,21 +2475,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2637,31 +2620,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2677,4 +2651,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implement optional soft line load limits
Improve eLLL_Can_Line3/eSoftLineLoadLimitCanInv to correctly work also in rMIP context
Remove left-over comments
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E0CA78E-D36B-490B-92E5-FDC45998C0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D8350F-3DE3-4527-B9FC-4382E5AC7586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="129">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -153,9 +153,6 @@
     <t>pCO2Cost</t>
   </si>
   <si>
-    <t>pEnableMaxLineLoad</t>
-  </si>
-  <si>
     <t>pEnableMinProdRESTech</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>Maximum angle difference</t>
   </si>
   <si>
-    <t>Enable maximum line load</t>
-  </si>
-  <si>
     <t>Maximum line load</t>
   </si>
   <si>
@@ -445,6 +439,18 @@
   </si>
   <si>
     <t>p2ndResDW</t>
+  </si>
+  <si>
+    <t>pEnableSoftLineLoadLimits</t>
+  </si>
+  <si>
+    <t>Enable soft line load limits</t>
+  </si>
+  <si>
+    <t>[0-100%]</t>
+  </si>
+  <si>
+    <t>Scales pMax, rest to 100% is soft limit</t>
   </si>
 </sst>
 </file>
@@ -662,481 +668,467 @@
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
   </cellStyles>
-  <dxfs count="72">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
+  <dxfs count="70">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
       </font>
     </dxf>
     <dxf>
@@ -1486,9 +1478,7 @@
   </sheetPr>
   <dimension ref="B1:H125"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1505,68 +1495,68 @@
   <sheetData>
     <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E3" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="H3" s="11" t="s">
         <v>94</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>81</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="8" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="9" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>1</v>
@@ -1580,19 +1570,19 @@
         <v>10000</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>4</v>
@@ -1606,13 +1596,13 @@
         <v>100</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1622,7 +1612,7 @@
     </row>
     <row r="16" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>0</v>
@@ -1630,19 +1620,19 @@
     </row>
     <row r="17" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C17" s="9">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1651,26 +1641,26 @@
     </row>
     <row r="19" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1678,10 +1668,10 @@
     </row>
     <row r="23" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1697,10 +1687,10 @@
     </row>
     <row r="26" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1716,15 +1706,15 @@
     </row>
     <row r="29" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C30" s="9">
         <v>180</v>
@@ -1735,18 +1725,18 @@
     </row>
     <row r="32" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
-        <v>41</v>
+        <v>126</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
-        <v>29</v>
+        <v>125</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1754,10 +1744,10 @@
     </row>
     <row r="35" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>5</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1767,13 +1757,16 @@
       <c r="C36" s="10">
         <v>0.7</v>
       </c>
+      <c r="E36" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="37" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="3"/>
     </row>
     <row r="38" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>1</v>
@@ -1781,7 +1774,7 @@
     </row>
     <row r="39" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="9">
         <v>100</v>
@@ -1792,12 +1785,12 @@
     </row>
     <row r="41" spans="2:5" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B41" s="7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B42" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>5</v>
@@ -1816,21 +1809,21 @@
     </row>
     <row r="45" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="46" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1838,15 +1831,15 @@
     </row>
     <row r="48" spans="2:5" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B49" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C49" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1862,7 +1855,7 @@
     </row>
     <row r="52" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C52" s="8" t="s">
         <v>20</v>
@@ -1878,7 +1871,7 @@
     </row>
     <row r="55" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>22</v>
@@ -1894,7 +1887,7 @@
     </row>
     <row r="58" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>22</v>
@@ -1910,12 +1903,12 @@
     </row>
     <row r="61" spans="2:3" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B61" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="63" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C63" s="8" t="s">
         <v>5</v>
@@ -1931,15 +1924,15 @@
     </row>
     <row r="66" spans="2:5" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="67" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C67" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="68" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1952,7 +1945,7 @@
     </row>
     <row r="70" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C70" s="8" t="s">
         <v>14</v>
@@ -1960,7 +1953,7 @@
     </row>
     <row r="71" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B71" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C71" s="9">
         <v>50</v>
@@ -1968,7 +1961,7 @@
     </row>
     <row r="73" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B73" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C73" s="8" t="s">
         <v>7</v>
@@ -1984,7 +1977,7 @@
     </row>
     <row r="76" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C76" s="8" t="s">
         <v>16</v>
@@ -2003,58 +1996,58 @@
     </row>
     <row r="79" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C79" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="80" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B80" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C80" s="9">
         <v>10</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="83" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B83" s="5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C83" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="84" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B84" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C84" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B86" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="87" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B87" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C87" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="88" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2068,7 +2061,7 @@
     <row r="89" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="90" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B90" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C90" s="8" t="s">
         <v>1</v>
@@ -2076,33 +2069,33 @@
     </row>
     <row r="91" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B91" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C91" s="9">
         <f>0.1*10^-3</f>
         <v>1E-4</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="93" spans="2:8" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B93" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="94" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B94" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C94" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="95" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2118,34 +2111,34 @@
     </row>
     <row r="97" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B97" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C97" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="98" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B98" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C98" s="9">
         <v>16</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="100" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B100" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C100" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="101" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B101" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C101" s="6" t="s">
         <v>11</v>
@@ -2153,39 +2146,39 @@
     </row>
     <row r="103" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B103" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C103" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="104" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B104" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C104" s="6" t="s">
         <v>18</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="106" spans="2:5" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B106" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="107" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B107" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C107" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="108" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B108" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C108" s="6" t="s">
         <v>11</v>
@@ -2193,10 +2186,10 @@
     </row>
     <row r="110" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B110" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C110" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="111" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2209,12 +2202,12 @@
     </row>
     <row r="113" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B113" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="114" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B114" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C114" s="8" t="s">
         <v>5</v>
@@ -2228,13 +2221,13 @@
         <v>0.03</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="116" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2243,7 +2236,7 @@
     </row>
     <row r="117" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B117" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C117" s="8" t="s">
         <v>5</v>
@@ -2251,19 +2244,19 @@
     </row>
     <row r="118" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B118" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C118" s="10">
         <v>0.03</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="119" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2272,7 +2265,7 @@
     </row>
     <row r="120" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B120" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C120" s="8" t="s">
         <v>0</v>
@@ -2280,16 +2273,16 @@
     </row>
     <row r="121" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B121" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C121" s="13">
         <v>0.2</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G121" s="1" t="s">
         <v>0</v>
@@ -2301,7 +2294,7 @@
     </row>
     <row r="123" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B123" s="5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C123" s="8" t="s">
         <v>0</v>
@@ -2309,16 +2302,16 @@
     </row>
     <row r="124" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B124" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C124" s="13">
         <v>0.2</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>0</v>
@@ -2330,291 +2323,283 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="71" priority="7" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="7" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="8" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="cellIs" dxfId="69" priority="17" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="17" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="18" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C12">
-    <cfRule type="cellIs" dxfId="67" priority="77" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="78" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="65" priority="78" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="77" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:C15">
-    <cfRule type="cellIs" dxfId="65" priority="75" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="76" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="63" priority="76" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="75" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:C18">
-    <cfRule type="cellIs" dxfId="63" priority="73" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="74" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="61" priority="74" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="73" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="cellIs" dxfId="59" priority="87" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="88" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="cellIs" dxfId="57" priority="66" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="65" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27 C30">
+    <cfRule type="cellIs" dxfId="55" priority="64" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="63" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="cellIs" dxfId="53" priority="62" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="61" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C36">
+    <cfRule type="cellIs" dxfId="51" priority="60" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="59" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C39">
+    <cfRule type="cellIs" dxfId="49" priority="58" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="57" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
+    <cfRule type="cellIs" dxfId="47" priority="56" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="55" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46">
+    <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="53" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C50">
+    <cfRule type="cellIs" dxfId="43" priority="52" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="51" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="cellIs" dxfId="41" priority="50" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="49" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
+    <cfRule type="cellIs" dxfId="39" priority="48" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="47" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59">
+    <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="45" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C64">
+    <cfRule type="cellIs" dxfId="35" priority="44" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="43" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C68">
+    <cfRule type="cellIs" dxfId="33" priority="41" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="42" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71">
+    <cfRule type="cellIs" dxfId="31" priority="40" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="39" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C74">
+    <cfRule type="cellIs" dxfId="29" priority="38" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="37" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C77">
+    <cfRule type="cellIs" dxfId="27" priority="36" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="35" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C80">
+    <cfRule type="cellIs" dxfId="25" priority="16" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C84">
+    <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="31" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C88:C89">
+    <cfRule type="cellIs" dxfId="21" priority="30" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="29" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C91">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C95">
+    <cfRule type="cellIs" dxfId="17" priority="28" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="27" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C98">
+    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C101 C104">
+    <cfRule type="cellIs" dxfId="13" priority="22" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="21" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C108">
+    <cfRule type="cellIs" dxfId="11" priority="26" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="25" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C111">
+    <cfRule type="cellIs" dxfId="9" priority="24" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="23" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C115:C116">
-    <cfRule type="cellIs" dxfId="61" priority="71" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="72" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="7" priority="72" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="71" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C118:C119">
-    <cfRule type="cellIs" dxfId="59" priority="9" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="10" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="57" priority="87" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="88" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
-    <cfRule type="cellIs" dxfId="55" priority="65" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="66" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C27 C30">
-    <cfRule type="cellIs" dxfId="53" priority="63" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="64" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="51" priority="61" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="62" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="49" priority="59" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="60" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C39">
-    <cfRule type="cellIs" dxfId="47" priority="57" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="58" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
-    <cfRule type="cellIs" dxfId="45" priority="55" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="56" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
-    <cfRule type="cellIs" dxfId="43" priority="53" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="54" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="cellIs" dxfId="41" priority="51" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="52" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
-    <cfRule type="cellIs" dxfId="39" priority="49" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="50" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
-    <cfRule type="cellIs" dxfId="37" priority="47" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="48" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
-    <cfRule type="cellIs" dxfId="35" priority="45" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="46" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="33" priority="43" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="44" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C68">
-    <cfRule type="cellIs" dxfId="31" priority="41" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="42" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C71">
-    <cfRule type="cellIs" dxfId="29" priority="39" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="40" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C74">
-    <cfRule type="cellIs" dxfId="27" priority="37" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="38" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C77">
-    <cfRule type="cellIs" dxfId="25" priority="35" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="36" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C80">
-    <cfRule type="cellIs" dxfId="23" priority="15" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="16" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C84">
-    <cfRule type="cellIs" dxfId="21" priority="31" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="32" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C88:C89">
-    <cfRule type="cellIs" dxfId="19" priority="29" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="30" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C91">
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C95">
-    <cfRule type="cellIs" dxfId="15" priority="27" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="28" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C101 C104">
-    <cfRule type="cellIs" dxfId="11" priority="21" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="22" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C108">
-    <cfRule type="cellIs" dxfId="9" priority="25" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="26" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C111">
-    <cfRule type="cellIs" dxfId="7" priority="23" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C121:C122">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C125">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C124">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C124:C125">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -2630,6 +2615,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2775,12 +2766,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2791,6 +2776,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2808,22 +2809,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Implement notEnforced and cyclic handling for min Up-/Down-time constr.
Update pyomo to 6.9.0
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D8350F-3DE3-4527-B9FC-4382E5AC7586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3A5F64-C215-4E1E-A150-B9524EA8C022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5835" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="135">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -451,6 +451,24 @@
   </si>
   <si>
     <t>Scales pMax, rest to 100% is soft limit</t>
+  </si>
+  <si>
+    <t>Constraint enforce type for border timesteps within p</t>
+  </si>
+  <si>
+    <t>[notEnforced, cyclic, markov]</t>
+  </si>
+  <si>
+    <t>pReprPeriodBorderType</t>
+  </si>
+  <si>
+    <t>cyclic</t>
+  </si>
+  <si>
+    <t>Minimum Up-/Down Time</t>
+  </si>
+  <si>
+    <t>How should constraints be enforced at border timesteps of repr. periods. Either, not enforced (=notEnforced), cyclically or using markov chains (from the transition matrix, which also means relaxing the binary form of affected variables)</t>
   </si>
 </sst>
 </file>
@@ -668,467 +686,481 @@
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
   </cellStyles>
-  <dxfs count="70">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
+  <dxfs count="72">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
       </font>
     </dxf>
     <dxf>
@@ -1476,9 +1508,11 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:H125"/>
+  <dimension ref="B1:H128"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="F129" sqref="F129"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2321,24 +2355,59 @@
       <c r="B125" s="3"/>
       <c r="C125"/>
     </row>
+    <row r="126" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B126" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B127" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C127" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B128" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C128" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F128" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="69" priority="7" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="9" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="10" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="cellIs" dxfId="67" priority="17" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="19" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="20" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C12">
+    <cfRule type="cellIs" dxfId="67" priority="79" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="80" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C14:C15">
     <cfRule type="cellIs" dxfId="65" priority="78" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2346,7 +2415,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:C15">
+  <conditionalFormatting sqref="C17:C18">
     <cfRule type="cellIs" dxfId="63" priority="76" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2354,23 +2423,23 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17:C18">
-    <cfRule type="cellIs" dxfId="61" priority="74" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="73" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="59" priority="87" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="89" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="90" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
+    <cfRule type="cellIs" dxfId="59" priority="68" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="67" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27 C30">
     <cfRule type="cellIs" dxfId="57" priority="66" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2378,7 +2447,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27 C30">
+  <conditionalFormatting sqref="C33">
     <cfRule type="cellIs" dxfId="55" priority="64" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2386,7 +2455,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
+  <conditionalFormatting sqref="C36">
     <cfRule type="cellIs" dxfId="53" priority="62" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2394,15 +2463,15 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="51" priority="60" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="59" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C39">
+    <cfRule type="cellIs" dxfId="51" priority="59" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="60" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
     <cfRule type="cellIs" dxfId="49" priority="58" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2410,7 +2479,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
+  <conditionalFormatting sqref="C46">
     <cfRule type="cellIs" dxfId="47" priority="56" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2418,7 +2487,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
+  <conditionalFormatting sqref="C50">
     <cfRule type="cellIs" dxfId="45" priority="54" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2426,15 +2495,15 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
-    <cfRule type="cellIs" dxfId="43" priority="52" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="51" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C53">
+    <cfRule type="cellIs" dxfId="43" priority="51" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="52" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C56">
     <cfRule type="cellIs" dxfId="41" priority="50" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2442,7 +2511,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C59">
     <cfRule type="cellIs" dxfId="39" priority="48" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2450,7 +2519,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
+  <conditionalFormatting sqref="C64">
     <cfRule type="cellIs" dxfId="37" priority="46" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2458,23 +2527,23 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
-    <cfRule type="cellIs" dxfId="35" priority="44" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="43" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C68">
-    <cfRule type="cellIs" dxfId="33" priority="41" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="43" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="44" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71">
+    <cfRule type="cellIs" dxfId="33" priority="42" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="41" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C74">
     <cfRule type="cellIs" dxfId="31" priority="40" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2482,7 +2551,7 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C74">
+  <conditionalFormatting sqref="C77">
     <cfRule type="cellIs" dxfId="29" priority="38" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2490,23 +2559,23 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C77">
-    <cfRule type="cellIs" dxfId="27" priority="36" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="35" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C80">
-    <cfRule type="cellIs" dxfId="25" priority="16" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="18" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="17" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C84">
+    <cfRule type="cellIs" dxfId="25" priority="33" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="34" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C88:C89">
     <cfRule type="cellIs" dxfId="23" priority="32" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2514,47 +2583,47 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C88:C89">
-    <cfRule type="cellIs" dxfId="21" priority="30" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="29" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C91">
-    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="14" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C95">
-    <cfRule type="cellIs" dxfId="17" priority="28" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="30" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="29" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C101 C104">
-    <cfRule type="cellIs" dxfId="13" priority="22" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="24" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="23" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C108">
+    <cfRule type="cellIs" dxfId="13" priority="28" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="27" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C111">
     <cfRule type="cellIs" dxfId="11" priority="26" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
@@ -2562,44 +2631,44 @@
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C111">
-    <cfRule type="cellIs" dxfId="9" priority="24" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="23" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C115:C116">
-    <cfRule type="cellIs" dxfId="7" priority="72" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="71" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="9" priority="73" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="74" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C118:C119">
-    <cfRule type="cellIs" dxfId="5" priority="9" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="10" operator="equal">
-      <formula>"Yes"</formula>
+    <cfRule type="cellIs" dxfId="7" priority="12" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="11" operator="equal">
+      <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C121:C122">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="equal">
       <formula>"No"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C124:C125">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"No"</formula>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C128">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
@@ -2607,7 +2676,7 @@
       <formula1>"No, Yes"</formula1>
     </dataValidation>
     <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C12 C15 C18 C116 C6 C119 C122 C125" xr:uid="{87C6F772-FD4B-9449-B9E7-DA0FF0A031BB}"/>
-    <dataValidation operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C115 C64 C36 C43 C118 C121 C124" xr:uid="{2B929D69-0393-BA4C-AFD3-02F233DB330E}"/>
+    <dataValidation operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C115 C64 C36 C43 C118 C121 C124 C128" xr:uid="{2B929D69-0393-BA4C-AFD3-02F233DB330E}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2615,12 +2684,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2766,6 +2829,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2776,22 +2845,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2809,6 +2862,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Implement markov-handling of border timesteps for repr.-periods
Adjust calculation of transitionMatrixRelative to account for 'to' and 'from' differently
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB3A5F64-C215-4E1E-A150-B9524EA8C022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF29570-56C5-4C84-87D1-AA3CE2DDC0E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5835" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -462,13 +462,13 @@
     <t>pReprPeriodBorderType</t>
   </si>
   <si>
-    <t>cyclic</t>
-  </si>
-  <si>
     <t>Minimum Up-/Down Time</t>
   </si>
   <si>
     <t>How should constraints be enforced at border timesteps of repr. periods. Either, not enforced (=notEnforced), cyclically or using markov chains (from the transition matrix, which also means relaxing the binary form of affected variables)</t>
+  </si>
+  <si>
+    <t>markov</t>
   </si>
 </sst>
 </file>
@@ -1510,8 +1510,8 @@
   </sheetPr>
   <dimension ref="B1:H128"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="F129" sqref="F129"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="C128" sqref="C128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2357,7 +2357,7 @@
     </row>
     <row r="126" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B126" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="127" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2373,10 +2373,10 @@
         <v>131</v>
       </c>
       <c r="C128" s="10" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>130</v>

</xml_diff>

<commit_message>
Add  SOCP parameters, variables and  a few constraints
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CABD84-5D25-4357-8B81-4C4980B6CFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{911A4AD2-AF75-41BB-84C5-586E1258A9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5325" yWindow="3840" windowWidth="28800" windowHeight="15030" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Parameters" sheetId="121" r:id="rId1"/>
@@ -724,12 +724,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
+    <cellStyle name="Ausgabe" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
     <cellStyle name="Hervorhebung" xfId="3" xr:uid="{8678E36F-C265-4DFE-9FC6-523CB5A8AE55}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{18929256-C3F4-489D-8BCE-E323A983834F}"/>
-    <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="8" builtinId="5"/>
+    <cellStyle name="Prozent" xfId="8" builtinId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Standard 2" xfId="5" xr:uid="{5DF4A97E-8529-4A9B-8CDD-1ED3E5DC1118}"/>
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
@@ -1558,11 +1558,11 @@
   </sheetPr>
   <dimension ref="B1:H144"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="51" style="1" customWidth="1"/>
@@ -2851,18 +2851,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3012,6 +3012,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3023,14 +3031,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixed 11592 constraint coefficient errors. 0 Remaining
Still doesn't solve >(
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46980BE0-5574-4AA9-BAE2-73BE6678B40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A3C22D-8133-444E-A48E-DB39F283F159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="78750" yWindow="7220" windowWidth="28800" windowHeight="15240" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="75990" yWindow="5470" windowWidth="28800" windowHeight="15240" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Parameters" sheetId="121" r:id="rId1"/>
@@ -516,7 +516,7 @@
     <t>How should constraints be enforced at edges of repr. periods. Either, not enforced (=notEnforced), cyclically or using markov chains (from the transition matrix)</t>
   </si>
   <si>
-    <t>notEnforced</t>
+    <t>cyclic</t>
   </si>
 </sst>
 </file>
@@ -1559,7 +1559,7 @@
   <dimension ref="B1:H144"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="E145" sqref="E145"/>
+      <selection activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.86328125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -2851,12 +2851,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -3002,6 +2996,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3012,22 +3012,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3045,6 +3029,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fixed the Fixed SOCP P and Q Power Balance(Finally Works)
Fixed eSOCP_QMinOut1 and eSOCP_QMinOut2
Added Bool for pEnable SOCP again
Add GAMS objective value extraction in the compare tool for MIP
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77144BB2-B191-46C7-A1DA-08E634B80E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41B927B-9F52-4EF9-AE96-3C5CEA48EE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34450" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="23226" windowHeight="13866" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Parameters" sheetId="121" r:id="rId1"/>
@@ -1558,8 +1558,8 @@
   </sheetPr>
   <dimension ref="B1:H144"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.86328125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
saved UNDO information for reset changes and discarded files
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11110318-CF35-41E7-9438-129A1B7162E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AE6FC8-E075-43FA-A318-7D052B8A77F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="23226" windowHeight="13866" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1558,8 +1558,8 @@
   </sheetPr>
   <dimension ref="B1:H144"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.86328125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -1858,7 +1858,7 @@
         <v>9</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
@@ -2851,18 +2851,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3012,6 +3012,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -3023,14 +3031,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Move links data to separate folder
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\GIT\LEGO-Pyomo\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D989434F-2261-4ABE-98E6-677CC43536FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601E25C3-0C7B-49B4-884D-9E815CDC6B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4170" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="94">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -346,15 +346,6 @@
   </si>
   <si>
     <t>cyclic</t>
-  </si>
-  <si>
-    <t>Enable Links?</t>
-  </si>
-  <si>
-    <t>pEnableLinks</t>
-  </si>
-  <si>
-    <t>Enable Links</t>
   </si>
 </sst>
 </file>
@@ -562,17 +553,283 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Ausgabe" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
     <cellStyle name="Hervorhebung" xfId="3" xr:uid="{8678E36F-C265-4DFE-9FC6-523CB5A8AE55}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{18929256-C3F4-489D-8BCE-E323A983834F}"/>
-    <cellStyle name="Prozent" xfId="8" builtinId="5"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="8" builtinId="5"/>
     <cellStyle name="Standard 2" xfId="5" xr:uid="{5DF4A97E-8529-4A9B-8CDD-1ED3E5DC1118}"/>
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="72">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF4E9C49"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFB90135"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1128,13 +1385,11 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:H82"/>
+  <dimension ref="B1:H79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B15" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="51" style="1" customWidth="1"/>
@@ -1390,221 +1645,227 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B31" s="3"/>
-      <c r="C31"/>
-    </row>
-    <row r="32" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="C32" s="8" t="s">
+    <row r="32" spans="2:6" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C33" s="6" t="s">
+    <row r="34" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B34" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E34" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B36" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B37" s="3" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C37" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B42" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="9">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B45" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B46" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="8" t="s">
+    </row>
+    <row r="47" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B48" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B49" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B51" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B52" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C52" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="2:7" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B54" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B55" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40" s="6" t="s">
+    <row r="56" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B56" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="9">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C46" s="9">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="47" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B48" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B49" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C52" s="10">
-        <v>0.7</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C55" s="9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="56" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="3"/>
-    </row>
-    <row r="57" spans="2:5" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B57" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="58" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B58" s="5" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B59" s="3" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="61" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B61" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="62" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C62" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E62" s="1" t="s">
+      <c r="E59" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="2:5" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B64" s="7" t="s">
+    <row r="61" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B61" s="7" t="s">
         <v>59</v>
       </c>
+    </row>
+    <row r="62" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B62" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B63" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B64" s="3"/>
+      <c r="C64"/>
     </row>
     <row r="65" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B65" s="5" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>5</v>
@@ -1612,16 +1873,16 @@
     </row>
     <row r="66" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B66" s="3" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="C66" s="10">
         <v>0.03</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>48</v>
@@ -1633,27 +1894,27 @@
     </row>
     <row r="68" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B68" s="5" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B69" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C69" s="10">
-        <v>0.03</v>
+        <v>61</v>
+      </c>
+      <c r="C69" s="13">
+        <v>0.2</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>48</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1662,7 +1923,7 @@
     </row>
     <row r="71" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B71" s="5" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>0</v>
@@ -1670,16 +1931,16 @@
     </row>
     <row r="72" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B72" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C72" s="13">
         <v>0.2</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>0</v>
@@ -1689,43 +1950,36 @@
       <c r="B73" s="3"/>
       <c r="C73"/>
     </row>
-    <row r="74" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B74" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C74" s="8" t="s">
-        <v>0</v>
+    <row r="74" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B74" s="7" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="75" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B75" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C75" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G75" s="1" t="s">
-        <v>0</v>
+      <c r="B75" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="76" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B76" s="3"/>
-      <c r="C76"/>
-    </row>
-    <row r="77" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B77" s="7" t="s">
-        <v>88</v>
+      <c r="B76" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="78" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B78" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>71</v>
@@ -1733,154 +1987,132 @@
     </row>
     <row r="79" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B79" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>93</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="81" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B81" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="82" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B82" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C82" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C6">
-    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="39" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="40" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="cellIs" dxfId="31" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="99" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="100" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C12">
-    <cfRule type="cellIs" dxfId="29" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="97" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="98" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:C34">
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
+  <conditionalFormatting sqref="C14:C31">
+    <cfRule type="cellIs" dxfId="65" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="4" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C34">
+    <cfRule type="cellIs" dxfId="63" priority="109" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="110" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="25" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="61" priority="87" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="60" priority="88" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
-    <cfRule type="cellIs" dxfId="23" priority="87" operator="equal">
+  <conditionalFormatting sqref="C40 C43">
+    <cfRule type="cellIs" dxfId="59" priority="85" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="86" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43 C46">
-    <cfRule type="cellIs" dxfId="21" priority="85" operator="equal">
+  <conditionalFormatting sqref="C46">
+    <cfRule type="cellIs" dxfId="57" priority="83" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="84" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="19" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="81" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="82" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="cellIs" dxfId="17" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="79" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="80" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
-    <cfRule type="cellIs" dxfId="15" priority="79" operator="equal">
+  <conditionalFormatting sqref="C56 C59">
+    <cfRule type="cellIs" dxfId="17" priority="43" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="44" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C59 C62">
-    <cfRule type="cellIs" dxfId="13" priority="43" operator="equal">
+  <conditionalFormatting sqref="C63:C64">
+    <cfRule type="cellIs" dxfId="11" priority="93" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="94" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66:C67">
-    <cfRule type="cellIs" dxfId="11" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="31" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="32" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C70">
-    <cfRule type="cellIs" dxfId="9" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="27" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="28" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C72:C73">
-    <cfRule type="cellIs" dxfId="7" priority="27" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="28" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C75:C76">
     <cfRule type="cellIs" dxfId="5" priority="23" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1888,7 +2120,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C79">
+  <conditionalFormatting sqref="C76">
     <cfRule type="cellIs" dxfId="3" priority="21" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1896,7 +2128,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C82">
+  <conditionalFormatting sqref="C79">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -1905,11 +2137,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C37 C40 C49 C59 C62 C27 C18 C24 C21 C30 C33" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C34 C37 C46 C56 C59 C27 C18 C24 C21 C30" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
       <formula1>"No, Yes"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C9 C12 C67 C70 C73 C76 C15:C34" xr:uid="{87C6F772-FD4B-9449-B9E7-DA0FF0A031BB}"/>
-    <dataValidation operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C66 C52 C69 C72 C75 C79 C82" xr:uid="{2B929D69-0393-BA4C-AFD3-02F233DB330E}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C9 C12 C64 C67 C70 C73 C15:C31" xr:uid="{87C6F772-FD4B-9449-B9E7-DA0FF0A031BB}"/>
+    <dataValidation operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C63 C49 C66 C69 C72 C76 C79" xr:uid="{2B929D69-0393-BA4C-AFD3-02F233DB330E}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1926,6 +2158,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2071,12 +2309,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
@@ -2086,6 +2318,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2101,20 +2349,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update launch file to Links
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micha\Desktop\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601E25C3-0C7B-49B4-884D-9E815CDC6B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1D6795-3CB9-40CA-B84D-AC74B318148D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4170" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="97">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -346,6 +346,15 @@
   </si>
   <si>
     <t>cyclic</t>
+  </si>
+  <si>
+    <t>Enable Links?</t>
+  </si>
+  <si>
+    <t>pEnableLinks</t>
+  </si>
+  <si>
+    <t>Enable Links</t>
   </si>
 </sst>
 </file>
@@ -553,283 +562,17 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
+    <cellStyle name="Ausgabe" xfId="2" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Data" xfId="1" xr:uid="{226E918E-BB32-45FB-8600-16B83FFE7285}"/>
     <cellStyle name="Hervorhebung" xfId="3" xr:uid="{8678E36F-C265-4DFE-9FC6-523CB5A8AE55}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Normal 2" xfId="4" xr:uid="{18929256-C3F4-489D-8BCE-E323A983834F}"/>
-    <cellStyle name="Output" xfId="2" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="8" builtinId="5"/>
+    <cellStyle name="Prozent" xfId="8" builtinId="5"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Standard 2" xfId="5" xr:uid="{5DF4A97E-8529-4A9B-8CDD-1ED3E5DC1118}"/>
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
   </cellStyles>
-  <dxfs count="72">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
+  <dxfs count="34">
     <dxf>
       <font>
         <b/>
@@ -1385,11 +1128,13 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:H79"/>
+  <dimension ref="B1:H82"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="51" style="1" customWidth="1"/>
@@ -1645,227 +1390,221 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="2:6" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="7" t="s">
+    <row r="31" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="3"/>
+      <c r="C31"/>
+    </row>
+    <row r="32" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B35" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="5" t="s">
+    <row r="36" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B34" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B37" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B39" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="5" t="s">
+    <row r="41" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B42" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C42" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="40" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="3" t="s">
+    <row r="43" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B43" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C43" s="9">
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="5" t="s">
+    <row r="44" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B45" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C45" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="43" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="3" t="s">
+    <row r="46" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B46" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C43" s="9">
+      <c r="C46" s="9">
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="5" t="s">
+    <row r="47" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B48" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C48" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="3" t="s">
+    <row r="49" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B49" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="6" t="s">
+      <c r="C49" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B48" s="5" t="s">
+    <row r="50" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B51" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C51" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="49" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B49" s="3" t="s">
+    <row r="52" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B52" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C49" s="10">
+      <c r="C52" s="10">
         <v>0.7</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E52" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="50" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="5" t="s">
+    <row r="53" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B54" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C54" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="3" t="s">
+    <row r="55" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B55" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C52" s="9">
+      <c r="C55" s="9">
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="2:7" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="7" t="s">
+    <row r="56" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="2:5" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B57" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B55" s="5" t="s">
+    <row r="58" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B58" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="56" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B56" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C56" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B58" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="C58" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B61" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B62" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C62" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E62" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B61" s="7" t="s">
+    <row r="64" spans="2:5" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B64" s="7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="62" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B62" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="63" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B63" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C63" s="10">
-        <v>0.03</v>
-      </c>
-      <c r="E63" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F63" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="64" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B64" s="3"/>
-      <c r="C64"/>
     </row>
     <row r="65" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B65" s="5" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C65" s="8" t="s">
         <v>5</v>
@@ -1873,16 +1612,16 @@
     </row>
     <row r="66" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B66" s="3" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C66" s="10">
         <v>0.03</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>48</v>
@@ -1894,27 +1633,27 @@
     </row>
     <row r="68" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B68" s="5" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="C68" s="8" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B69" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C69" s="13">
-        <v>0.2</v>
+        <v>66</v>
+      </c>
+      <c r="C69" s="10">
+        <v>0.03</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
     </row>
     <row r="70" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -1923,7 +1662,7 @@
     </row>
     <row r="71" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B71" s="5" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C71" s="8" t="s">
         <v>0</v>
@@ -1931,16 +1670,16 @@
     </row>
     <row r="72" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B72" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C72" s="13">
         <v>0.2</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>0</v>
@@ -1950,36 +1689,43 @@
       <c r="B73" s="3"/>
       <c r="C73"/>
     </row>
-    <row r="74" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B74" s="7" t="s">
+    <row r="74" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B74" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B75" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C75" s="13">
+        <v>0.2</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G75" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B76" s="3"/>
+      <c r="C76"/>
+    </row>
+    <row r="77" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B77" s="7" t="s">
         <v>88</v>
-      </c>
-    </row>
-    <row r="75" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B75" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C75" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="76" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B76" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C76" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="G76" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="78" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B78" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C78" s="8" t="s">
         <v>71</v>
@@ -1987,108 +1733,130 @@
     </row>
     <row r="79" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B79" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>93</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>71</v>
       </c>
     </row>
+    <row r="81" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B81" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B82" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="C5:C6">
-    <cfRule type="cellIs" dxfId="71" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="39" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="40" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="cellIs" dxfId="69" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="99" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="100" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C12">
-    <cfRule type="cellIs" dxfId="67" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="97" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="98" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:C31">
-    <cfRule type="cellIs" dxfId="65" priority="3" operator="equal">
+  <conditionalFormatting sqref="C14:C34">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="4" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="63" priority="109" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="61" priority="87" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="109" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="110" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40 C43">
-    <cfRule type="cellIs" dxfId="59" priority="85" operator="equal">
+  <conditionalFormatting sqref="C40">
+    <cfRule type="cellIs" dxfId="23" priority="87" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="88" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
-    <cfRule type="cellIs" dxfId="57" priority="83" operator="equal">
+  <conditionalFormatting sqref="C43 C46">
+    <cfRule type="cellIs" dxfId="21" priority="85" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="86" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="55" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="83" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="84" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C52">
-    <cfRule type="cellIs" dxfId="53" priority="79" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="81" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="82" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56 C59">
-    <cfRule type="cellIs" dxfId="17" priority="43" operator="equal">
+  <conditionalFormatting sqref="C55">
+    <cfRule type="cellIs" dxfId="15" priority="79" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="80" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63:C64">
+  <conditionalFormatting sqref="C59 C62">
+    <cfRule type="cellIs" dxfId="13" priority="43" operator="equal">
+      <formula>"No"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="44" operator="equal">
+      <formula>"Yes"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C66:C67">
     <cfRule type="cellIs" dxfId="11" priority="93" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -2096,7 +1864,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C66:C67">
+  <conditionalFormatting sqref="C69:C70">
     <cfRule type="cellIs" dxfId="9" priority="31" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -2104,7 +1872,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C69:C70">
+  <conditionalFormatting sqref="C72:C73">
     <cfRule type="cellIs" dxfId="7" priority="27" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -2112,7 +1880,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C72:C73">
+  <conditionalFormatting sqref="C75:C76">
     <cfRule type="cellIs" dxfId="5" priority="23" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -2120,7 +1888,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C76">
+  <conditionalFormatting sqref="C79">
     <cfRule type="cellIs" dxfId="3" priority="21" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -2128,7 +1896,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C79">
+  <conditionalFormatting sqref="C82">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -2137,11 +1905,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C34 C37 C46 C56 C59 C27 C18 C24 C21 C30" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C37 C40 C49 C59 C62 C27 C18 C24 C21 C30 C33" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
       <formula1>"No, Yes"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C9 C12 C64 C67 C70 C73 C15:C31" xr:uid="{87C6F772-FD4B-9449-B9E7-DA0FF0A031BB}"/>
-    <dataValidation operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C63 C49 C66 C69 C72 C76 C79" xr:uid="{2B929D69-0393-BA4C-AFD3-02F233DB330E}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C9 C12 C67 C70 C73 C76 C15:C34" xr:uid="{87C6F772-FD4B-9449-B9E7-DA0FF0A031BB}"/>
+    <dataValidation operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C66 C52 C69 C72 C75 C79 C82" xr:uid="{2B929D69-0393-BA4C-AFD3-02F233DB330E}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2158,12 +1926,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2309,6 +2071,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
@@ -2318,22 +2086,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2349,4 +2101,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add new input files for storage and vres, remove separate ror files
Add model.sqlite and model.xlsx to .gitignore
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601E25C3-0C7B-49B4-884D-9E815CDC6B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A1DF8E-B785-42B1-94F1-D43326561C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4170" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34230" yWindow="-21705" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Parameters" sheetId="121" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="91">
   <si>
     <t>[p.u.]</t>
   </si>
@@ -282,12 +282,6 @@
     <t>[notEnforced, cyclic, markov]</t>
   </si>
   <si>
-    <t>Run-of-River</t>
-  </si>
-  <si>
-    <t>pEnableRoR</t>
-  </si>
-  <si>
     <t>Enable modules and load corresponding input files</t>
   </si>
   <si>
@@ -307,9 +301,6 @@
   </si>
   <si>
     <t>Enable VRES</t>
-  </si>
-  <si>
-    <t>Enable Run-Of-River</t>
   </si>
   <si>
     <t>Storage</t>
@@ -563,287 +554,7 @@
     <cellStyle name="Standard 3" xfId="6" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
     <cellStyle name="Standard 4" xfId="7" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
   </cellStyles>
-  <dxfs count="72">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF4E9C49"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFB90135"/>
-      </font>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <font>
         <b/>
@@ -1385,11 +1096,11 @@
   <sheetPr>
     <tabColor rgb="FF008080"/>
   </sheetPr>
-  <dimension ref="B1:H79"/>
+  <dimension ref="B1:H76"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="51" style="1" customWidth="1"/>
@@ -1402,12 +1113,12 @@
     <col min="9" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:8" s="2" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>13</v>
       </c>
@@ -1427,7 +1138,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>33</v>
       </c>
@@ -1435,7 +1146,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
         <v>34</v>
       </c>
@@ -1443,8 +1154,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>14</v>
       </c>
@@ -1452,7 +1163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
@@ -1469,8 +1180,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="10" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>15</v>
       </c>
@@ -1478,7 +1189,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>3</v>
       </c>
@@ -1495,12 +1206,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:8" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1508,7 +1219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
@@ -1525,594 +1236,563 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
       <c r="C15"/>
     </row>
-    <row r="16" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:8" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
       <c r="C19"/>
     </row>
-    <row r="20" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="5" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>
       <c r="C22"/>
     </row>
-    <row r="23" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
       <c r="C25"/>
     </row>
-    <row r="26" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="5" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="C27" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B28" s="3"/>
-      <c r="C28"/>
-    </row>
-    <row r="29" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B29" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B32" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="E31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="C34" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" s="9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="9">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C43" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E34" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B36" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C36" s="8" t="s">
+    </row>
+    <row r="44" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51" spans="2:7" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B37" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37" s="6" t="s">
+    <row r="53" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B39" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="9">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B42" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B43" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C43" s="9">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B45" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B46" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B48" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="49" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B49" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49" s="10">
-        <v>0.7</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B51" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B52" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C52" s="9">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="2:7" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B54" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="5" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="3" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B58" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="59" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B59" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C59" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E59" s="1" t="s">
+      <c r="E56" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B61" s="7" t="s">
+    <row r="58" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="62" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B60" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B61" s="3"/>
+      <c r="C61"/>
+    </row>
+    <row r="62" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="5" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="C62" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="3" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="C63" s="10">
         <v>0.03</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G63" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="3"/>
       <c r="C64"/>
     </row>
-    <row r="65" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="5" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="C65" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C66" s="10">
-        <v>0.03</v>
+        <v>61</v>
+      </c>
+      <c r="C66" s="13">
+        <v>0.2</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="67" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B67" s="3"/>
       <c r="C67"/>
     </row>
-    <row r="68" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="5" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="C68" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C69" s="13">
         <v>0.2</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G69" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B70" s="3"/>
       <c r="C70"/>
     </row>
-    <row r="71" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B71" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C71" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B72" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C72" s="13">
-        <v>0.2</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B73" s="3"/>
-      <c r="C73"/>
-    </row>
-    <row r="74" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B74" s="7" t="s">
+    <row r="71" spans="2:7" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="5" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="75" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="C72" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B73" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C73" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C75" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C76" s="10" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="78" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B78" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="79" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B79" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C79" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="C5:C6">
-    <cfRule type="cellIs" dxfId="71" priority="39" operator="equal">
+  <conditionalFormatting sqref="C5:C6 C14:C28">
+    <cfRule type="cellIs" dxfId="31" priority="39" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="40" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:C9">
-    <cfRule type="cellIs" dxfId="69" priority="99" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="99" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="100" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:C12">
-    <cfRule type="cellIs" dxfId="67" priority="97" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="97" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="98" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14:C31">
-    <cfRule type="cellIs" dxfId="65" priority="3" operator="equal">
+  <conditionalFormatting sqref="C31">
+    <cfRule type="cellIs" dxfId="25" priority="109" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="110" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34">
-    <cfRule type="cellIs" dxfId="63" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="87" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="88" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
-    <cfRule type="cellIs" dxfId="61" priority="87" operator="equal">
+  <conditionalFormatting sqref="C37 C40">
+    <cfRule type="cellIs" dxfId="21" priority="85" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="86" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40 C43">
-    <cfRule type="cellIs" dxfId="59" priority="85" operator="equal">
+  <conditionalFormatting sqref="C43">
+    <cfRule type="cellIs" dxfId="19" priority="83" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="84" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="cellIs" dxfId="57" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="81" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="82" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C49">
-    <cfRule type="cellIs" dxfId="55" priority="81" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="79" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="80" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
-    <cfRule type="cellIs" dxfId="53" priority="79" operator="equal">
+  <conditionalFormatting sqref="C53 C56">
+    <cfRule type="cellIs" dxfId="13" priority="43" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="80" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="44" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56 C59">
-    <cfRule type="cellIs" dxfId="17" priority="43" operator="equal">
+  <conditionalFormatting sqref="C60:C61">
+    <cfRule type="cellIs" dxfId="11" priority="93" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="94" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C63:C64">
-    <cfRule type="cellIs" dxfId="11" priority="93" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="31" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="32" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C66:C67">
-    <cfRule type="cellIs" dxfId="9" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="27" operator="equal">
       <formula>"No"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="28" operator="equal">
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C69:C70">
-    <cfRule type="cellIs" dxfId="7" priority="27" operator="equal">
-      <formula>"No"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="28" operator="equal">
-      <formula>"Yes"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C72:C73">
     <cfRule type="cellIs" dxfId="5" priority="23" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -2120,7 +1800,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C76">
+  <conditionalFormatting sqref="C73">
     <cfRule type="cellIs" dxfId="3" priority="21" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -2128,7 +1808,7 @@
       <formula>"Yes"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C79">
+  <conditionalFormatting sqref="C76">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"No"</formula>
     </cfRule>
@@ -2137,11 +1817,11 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C34 C37 C46 C56 C59 C27 C18 C24 C21 C30" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C31 C34 C43 C53 C56 C24 C18 C21 C27" xr:uid="{3037D345-D942-4EE1-9FD6-4C812B603C20}">
       <formula1>"No, Yes"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C9 C12 C64 C67 C70 C73 C15:C31" xr:uid="{87C6F772-FD4B-9449-B9E7-DA0FF0A031BB}"/>
-    <dataValidation operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C63 C49 C66 C69 C72 C76 C79" xr:uid="{2B929D69-0393-BA4C-AFD3-02F233DB330E}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C9 C12 C61 C64 C67 C70 C15:C28" xr:uid="{87C6F772-FD4B-9449-B9E7-DA0FF0A031BB}"/>
+    <dataValidation operator="greaterThan" showInputMessage="1" showErrorMessage="1" sqref="C60 C46 C63 C66 C69 C73 C76" xr:uid="{2B929D69-0393-BA4C-AFD3-02F233DB330E}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2158,12 +1838,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2309,6 +1983,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
@@ -2318,22 +1998,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2349,4 +2013,20 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implement new Import/Export logic and activate in example
</commit_message>
<xml_diff>
--- a/data/example/Power_Parameters.xlsx
+++ b/data/example/Power_Parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo2\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A658E7-62F7-4FD1-9B9B-EE98D50A0A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD86268-C279-4592-95AE-389334B73F2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33915" yWindow="-21810" windowWidth="38640" windowHeight="21120" tabRatio="958" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1352,7 +1352,7 @@
         <v>58</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>82</v>
@@ -1854,6 +1854,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1999,15 +2008,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2015,6 +2015,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2028,14 +2036,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>